<commit_message>
Providing a better Excel formatting
</commit_message>
<xml_diff>
--- a/CHAR.xlsx
+++ b/CHAR.xlsx
@@ -3578,9 +3578,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A137"/>
+  <dimension ref="A1:A136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -4022,248 +4024,248 @@
         <v>78</v>
       </c>
     </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="89" spans="1:1">
       <c r="A89" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="1" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="1" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="1" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="1" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="1" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="1" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="1" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" s="1" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="1" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="1" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="1" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="1" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="1" t="s">
-        <v>2</v>
+        <v>110</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1">
-      <c r="A137" s="1" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>